<commit_message>
lets see how this goes
</commit_message>
<xml_diff>
--- a/masks/code/TKIDModule_spreadsheet_20200624_AW_special.xlsx
+++ b/masks/code/TKIDModule_spreadsheet_20200624_AW_special.xlsx
@@ -1206,8 +1206,8 @@
     <col customWidth="1" max="1" min="1" width="17"/>
     <col customWidth="1" max="2" min="2" width="11"/>
     <col customWidth="1" max="3" min="3" width="44"/>
-    <col customWidth="1" max="4" min="4" width="21"/>
-    <col customWidth="1" max="5" min="5" width="10"/>
+    <col customWidth="1" max="4" min="4" width="8"/>
+    <col customWidth="1" max="5" min="5" width="9"/>
     <col customWidth="1" max="6" min="6" width="7"/>
     <col customWidth="1" max="7" min="7" width="7"/>
     <col customWidth="1" max="8" min="8" width="21"/>
@@ -1217,7 +1217,7 @@
     <col customWidth="1" max="12" min="12" width="6"/>
     <col customWidth="1" max="13" min="13" width="8"/>
     <col customWidth="1" max="14" min="14" width="8"/>
-    <col customWidth="1" max="15" min="15" width="21"/>
+    <col customWidth="1" max="15" min="15" width="20"/>
     <col customWidth="1" max="16" min="16" width="22"/>
     <col customWidth="1" max="17" min="17" width="6"/>
     <col customWidth="1" max="18" min="18" width="6"/>
@@ -4482,10 +4482,10 @@
         <v>54</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>5.68999</v>
+        <v>5.69</v>
       </c>
       <c r="E54" s="1" t="n">
-        <v>10.76401</v>
+        <v>10.764</v>
       </c>
       <c r="F54" s="1" t="n">
         <v>8.619999999999999</v>
@@ -4494,16 +4494,16 @@
         <v>0.8</v>
       </c>
       <c r="H54" s="1" t="n">
-        <v>1.37999</v>
+        <v>1.380000000000001</v>
       </c>
       <c r="I54" s="1" t="n">
-        <v>9.99999</v>
+        <v>10</v>
       </c>
       <c r="J54" s="1" t="n">
-        <v>11.15001</v>
+        <v>11.15</v>
       </c>
       <c r="K54" s="1" t="n">
-        <v>10.35001</v>
+        <v>10.35</v>
       </c>
       <c r="L54" s="1" t="n"/>
       <c r="M54" s="1" t="n">
@@ -4513,10 +4513,10 @@
         <v>-3.943</v>
       </c>
       <c r="O54" s="1" t="n">
-        <v>5.68999</v>
+        <v>5.69</v>
       </c>
       <c r="P54" s="1" t="n">
-        <v>14.70701</v>
+        <v>14.707</v>
       </c>
       <c r="Q54" s="1" t="n"/>
       <c r="R54" s="1" t="n"/>
@@ -4986,10 +4986,10 @@
         <v>63</v>
       </c>
       <c r="D61" s="1" t="n">
-        <v>-5.32001</v>
+        <v>-5.32</v>
       </c>
       <c r="E61" s="1" t="n">
-        <v>10.82001</v>
+        <v>10.82</v>
       </c>
       <c r="F61" s="1" t="n">
         <v>4.4</v>
@@ -4998,16 +4998,16 @@
         <v>0.6</v>
       </c>
       <c r="H61" s="1" t="n">
-        <v>-7.52001</v>
+        <v>-7.52</v>
       </c>
       <c r="I61" s="1" t="n">
-        <v>-3.12001</v>
+        <v>-3.12</v>
       </c>
       <c r="J61" s="1" t="n">
-        <v>11.12001</v>
+        <v>11.12</v>
       </c>
       <c r="K61" s="1" t="n">
-        <v>10.52001</v>
+        <v>10.52</v>
       </c>
       <c r="L61" s="1" t="n"/>
       <c r="M61" s="1" t="n">
@@ -5017,10 +5017,10 @@
         <v>3.916</v>
       </c>
       <c r="O61" s="1" t="n">
-        <v>-5.32001</v>
+        <v>-5.32</v>
       </c>
       <c r="P61" s="1" t="n">
-        <v>6.90401</v>
+        <v>6.904</v>
       </c>
       <c r="Q61" s="1" t="n"/>
       <c r="R61" s="1" t="n"/>
@@ -14850,10 +14850,10 @@
         <v>200</v>
       </c>
       <c r="D198" s="1" t="n">
-        <v>-6.19401</v>
+        <v>-6.194</v>
       </c>
       <c r="E198" s="1" t="n">
-        <v>10.16001</v>
+        <v>10.16</v>
       </c>
       <c r="F198" s="1" t="n">
         <v>4.892</v>
@@ -14862,16 +14862,16 @@
         <v>0.62</v>
       </c>
       <c r="H198" s="1" t="n">
-        <v>-8.64001</v>
+        <v>-8.640000000000001</v>
       </c>
       <c r="I198" s="1" t="n">
-        <v>-3.74801</v>
+        <v>-3.748</v>
       </c>
       <c r="J198" s="1" t="n">
-        <v>10.47001</v>
+        <v>10.47</v>
       </c>
       <c r="K198" s="1" t="n">
-        <v>9.850009999999999</v>
+        <v>9.85</v>
       </c>
       <c r="L198" s="1" t="n"/>
       <c r="M198" s="1" t="n">
@@ -14881,10 +14881,10 @@
         <v>3.916</v>
       </c>
       <c r="O198" s="1" t="n">
-        <v>-6.19401</v>
+        <v>-6.194</v>
       </c>
       <c r="P198" s="1" t="n">
-        <v>6.244009999999999</v>
+        <v>6.244</v>
       </c>
       <c r="Q198" s="1" t="n"/>
       <c r="R198" s="1" t="n"/>
@@ -14922,10 +14922,10 @@
         <v>200</v>
       </c>
       <c r="D199" s="1" t="n">
-        <v>-6.19401</v>
+        <v>-6.194</v>
       </c>
       <c r="E199" s="1" t="n">
-        <v>10.16001</v>
+        <v>10.16</v>
       </c>
       <c r="F199" s="1" t="n">
         <v>4.892</v>
@@ -14934,16 +14934,16 @@
         <v>0.62</v>
       </c>
       <c r="H199" s="1" t="n">
-        <v>-8.64001</v>
+        <v>-8.640000000000001</v>
       </c>
       <c r="I199" s="1" t="n">
-        <v>-3.74801</v>
+        <v>-3.748</v>
       </c>
       <c r="J199" s="1" t="n">
-        <v>10.47001</v>
+        <v>10.47</v>
       </c>
       <c r="K199" s="1" t="n">
-        <v>9.850009999999999</v>
+        <v>9.85</v>
       </c>
       <c r="L199" s="1" t="n"/>
       <c r="M199" s="1" t="n">
@@ -14953,10 +14953,10 @@
         <v>-3.916</v>
       </c>
       <c r="O199" s="1" t="n">
-        <v>-6.19401</v>
+        <v>-6.194</v>
       </c>
       <c r="P199" s="1" t="n">
-        <v>14.07601</v>
+        <v>14.076</v>
       </c>
       <c r="Q199" s="1" t="n"/>
       <c r="R199" s="1" t="n"/>
@@ -15141,7 +15141,7 @@
         <v>-4.25</v>
       </c>
       <c r="E202" s="1" t="n">
-        <v>-11.575</v>
+        <v>-11.55</v>
       </c>
       <c r="F202" s="1" t="n">
         <v>6.6</v>
@@ -15156,10 +15156,10 @@
         <v>-0.9500000000000002</v>
       </c>
       <c r="J202" s="1" t="n">
-        <v>-10.925</v>
+        <v>-10.9</v>
       </c>
       <c r="K202" s="1" t="n">
-        <v>-12.225</v>
+        <v>-12.2</v>
       </c>
       <c r="L202" s="1" t="n"/>
       <c r="M202" s="1" t="n">
@@ -15172,7 +15172,7 @@
         <v>-4.25</v>
       </c>
       <c r="P202" s="1" t="n">
-        <v>-11.575</v>
+        <v>-11.55</v>
       </c>
       <c r="Q202" s="1" t="n"/>
       <c r="R202" s="1" t="n"/>
@@ -18450,10 +18450,10 @@
         <v>233</v>
       </c>
       <c r="D248" s="1" t="n">
-        <v>5.35001</v>
+        <v>5.35</v>
       </c>
       <c r="E248" s="1" t="n">
-        <v>11.94999</v>
+        <v>11.95</v>
       </c>
       <c r="F248" s="1" t="n">
         <v>6.8</v>
@@ -18462,16 +18462,16 @@
         <v>1.5</v>
       </c>
       <c r="H248" s="1" t="n">
-        <v>1.95001</v>
+        <v>1.95</v>
       </c>
       <c r="I248" s="1" t="n">
-        <v>8.75001</v>
+        <v>8.75</v>
       </c>
       <c r="J248" s="1" t="n">
-        <v>12.69999</v>
+        <v>12.7</v>
       </c>
       <c r="K248" s="1" t="n">
-        <v>11.19999</v>
+        <v>11.2</v>
       </c>
       <c r="L248" s="1" t="n"/>
       <c r="M248" s="1" t="n">
@@ -18481,10 +18481,10 @@
         <v>0</v>
       </c>
       <c r="O248" s="1" t="n">
-        <v>5.35001</v>
+        <v>5.35</v>
       </c>
       <c r="P248" s="1" t="n">
-        <v>11.94999</v>
+        <v>11.95</v>
       </c>
       <c r="Q248" s="1" t="n"/>
       <c r="R248" s="1" t="n"/>
@@ -19602,10 +19602,10 @@
         <v>245</v>
       </c>
       <c r="D264" s="1" t="n">
-        <v>-3.10001</v>
+        <v>-3.1</v>
       </c>
       <c r="E264" s="1" t="n">
-        <v>11.62001</v>
+        <v>11.62</v>
       </c>
       <c r="F264" s="1" t="n">
         <v>10</v>
@@ -19614,16 +19614,16 @@
         <v>0.9</v>
       </c>
       <c r="H264" s="1" t="n">
-        <v>-8.100010000000001</v>
+        <v>-8.1</v>
       </c>
       <c r="I264" s="1" t="n">
-        <v>1.89999</v>
+        <v>1.9</v>
       </c>
       <c r="J264" s="1" t="n">
-        <v>12.07001</v>
+        <v>12.07</v>
       </c>
       <c r="K264" s="1" t="n">
-        <v>11.17001</v>
+        <v>11.17</v>
       </c>
       <c r="L264" s="1" t="n"/>
       <c r="M264" s="1" t="n">
@@ -19633,10 +19633,10 @@
         <v>-3.943</v>
       </c>
       <c r="O264" s="1" t="n">
-        <v>-3.10001</v>
+        <v>-3.1</v>
       </c>
       <c r="P264" s="1" t="n">
-        <v>15.56301</v>
+        <v>15.563</v>
       </c>
       <c r="Q264" s="1" t="n"/>
       <c r="R264" s="1" t="n"/>
@@ -20322,10 +20322,10 @@
         <v>252</v>
       </c>
       <c r="D274" s="1" t="n">
-        <v>-0.87001</v>
+        <v>-0.87</v>
       </c>
       <c r="E274" s="1" t="n">
-        <v>10.82001</v>
+        <v>10.82</v>
       </c>
       <c r="F274" s="1" t="n">
         <v>4.4</v>
@@ -20334,16 +20334,16 @@
         <v>0.6</v>
       </c>
       <c r="H274" s="1" t="n">
-        <v>-3.07001</v>
+        <v>-3.07</v>
       </c>
       <c r="I274" s="1" t="n">
-        <v>1.32999</v>
+        <v>1.33</v>
       </c>
       <c r="J274" s="1" t="n">
-        <v>11.12001</v>
+        <v>11.12</v>
       </c>
       <c r="K274" s="1" t="n">
-        <v>10.52001</v>
+        <v>10.52</v>
       </c>
       <c r="L274" s="1" t="n"/>
       <c r="M274" s="1" t="n">
@@ -20353,10 +20353,10 @@
         <v>-3.916</v>
       </c>
       <c r="O274" s="1" t="n">
-        <v>-0.87001</v>
+        <v>-0.87</v>
       </c>
       <c r="P274" s="1" t="n">
-        <v>14.73601</v>
+        <v>14.736</v>
       </c>
       <c r="Q274" s="1" t="n"/>
       <c r="R274" s="1" t="n"/>

</xml_diff>